<commit_message>
CARGA NOVEDADES OK - REPORTE OK - ACTUALIZA NOMINA OK
</commit_message>
<xml_diff>
--- a/Dotacion.xlsx
+++ b/Dotacion.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bbracco\Documents\Python\RRHH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F0AE5E32-65D2-403D-80A7-12DA13C2568F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65DC2E26-6C93-4F81-9FE0-23BD64D7373B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="000010F8-00001154-20220324-1820" sheetId="2" r:id="rId1"/>
@@ -3700,7 +3700,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4597,11 +4597,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C1143"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A1120" workbookViewId="0">
+      <selection activeCell="A1140" sqref="A1140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>